<commit_message>
added output field and edited version
added output field and edited version
</commit_message>
<xml_diff>
--- a/templates/community/CEPLAS-data/Genome_assembly_report.xlsx
+++ b/templates/community/CEPLAS-data/Genome_assembly_report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.0.1</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Description</t>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Term Accession Number (GENEPIO:0000091)</t>
+  </si>
+  <si>
+    <t>Output [Data]</t>
   </si>
 </sst>
 </file>
@@ -238,8 +241,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:P1" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:P1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:Q1" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:Q1">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -256,8 +259,9 @@
     <filterColumn colId="13" hiddenButton="1"/>
     <filterColumn colId="14" hiddenButton="1"/>
     <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="16">
+  <tableColumns count="17">
     <tableColumn id="1" name="Input [Data]" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Characteristic [contig N50]" totalsRowFunction="none"/>
     <tableColumn id="3" name="Term Source REF (OBI:0001941)" totalsRowFunction="none"/>
@@ -274,6 +278,7 @@
     <tableColumn id="14" name="Characteristic [assembly status]" totalsRowFunction="none"/>
     <tableColumn id="15" name="Term Source REF (GENEPIO:0000091)" totalsRowFunction="none"/>
     <tableColumn id="16" name="Term Accession Number (GENEPIO:0000091)" totalsRowFunction="none"/>
+    <tableColumn id="17" name="Output [Data]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -766,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -817,6 +822,9 @@
       </c>
       <c r="P1" t="s">
         <v>56</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>